<commit_message>
First stage on NUTS 2 analysis
</commit_message>
<xml_diff>
--- a/raw_data/eurostat/nuts2_emp_lfs_9908.xlsx
+++ b/raw_data/eurostat/nuts2_emp_lfs_9908.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aml/AutoEmp/raw_data/eurostat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827A0B63-88E3-6B43-8CEC-7847087988D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7D9EB3-104B-1B47-93CD-F0D69B252A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="-23680" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="148">
   <si>
     <t>Employment by sex, age, economic activity and NUTS 2 regions (1999-2008, NACE Rev. 1.1) (1 000) [lfst_r_lfe2en1__custom_12460587]</t>
   </si>
@@ -484,7 +484,10 @@
     <t>region</t>
   </si>
   <si>
-    <t>total_emp</t>
+    <t>total_emp_2001</t>
+  </si>
+  <si>
+    <t>AB</t>
   </si>
 </sst>
 </file>
@@ -595,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -663,12 +666,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1463,90 +1465,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2642,12 +2644,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -2656,6 +2652,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2754,90 +2756,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3925,12 +3927,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -3939,6 +3935,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4037,90 +4039,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -5208,12 +5210,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -5222,6 +5218,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5971,90 +5973,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -7142,12 +7144,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -7156,6 +7152,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7254,90 +7256,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -8425,12 +8427,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -8439,6 +8435,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8452,7 +8454,7 @@
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8530,10 +8532,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -8556,10 +8558,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -8588,22 +8590,22 @@
       <c r="B13" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" t="s">
         <v>146</v>
       </c>
-      <c r="D13" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" s="26" t="s">
+      <c r="D13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" t="s">
         <v>43</v>
       </c>
     </row>
@@ -9325,90 +9327,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -10496,12 +10498,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -10510,6 +10506,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10608,90 +10610,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -11787,12 +11789,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -11801,6 +11797,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11899,90 +11901,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -13070,12 +13072,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -13084,6 +13080,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13182,90 +13184,90 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="24" t="s">
+      <c r="D11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I11" s="24" t="s">
+      <c r="H11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="24" t="s">
+      <c r="J11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K11" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="L11" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M11" s="24" t="s">
+      <c r="L11" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M11" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="25" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E12" s="24" t="s">
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="H12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="I12" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="24" t="s">
+      <c r="J12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="L12" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="M12" s="24" t="s">
+      <c r="L12" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="25" t="s">
         <v>43</v>
       </c>
     </row>
@@ -14361,12 +14363,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="M12:N12"/>
     <mergeCell ref="G11:H11"/>
@@ -14375,6 +14371,12 @@
     <mergeCell ref="I12:J12"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="K12:L12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>